<commit_message>
modified:   Brighway/Libaries/LCA_plots.py 	modified:   Brighway/Libaries/__pycache__/LCA_plots.cpython-311.pyc 	modified:   Brighway/Libaries/__pycache__/life_cycle_assessment.cpython-311.pyc 	modified:   Brighway/Libaries/life_cycle_assessment.py 	deleted:    Brighway/Ofir/Ofir BE.ipynb 	modified:   Brighway/Ofir/Ofir.ipynb 	new file:   Brighway/Results/Ananas - CONSQ_recipe_unq.xlsx 	modified:   Brighway/Results/Lobster - CONSQ_recipe.xlsx 	new file:   Brighway/Results_ Ofir/GWP_life_stage_pr_scenario_CONSQ.jpg 	new file:   Brighway/Results_ Ofir/break_even_large_CONSQ.jpg 	new file:   Brighway/Results_ Ofir/break_even_small_CONSQ.jpg 	new file:   Brighway/Results_ Ofir/scaled_impact_score_multi_CONSQ_ReCiPe 2016 v1.03, endpoint (H).jpg 	new file:   Brighway/Results_ Ofir/scaled_impact_score_multi_CONSQ_ReCiPe 2016 v1.03, midpoint (H).jpg 	modified:   Brighway/Results_Ofir/break_even_large_CONSQ.jpg 	modified:   Brighway/Results_Ofir/break_even_small_CONSQ.jpg
</commit_message>
<xml_diff>
--- a/Brighway/Results/Lobster - CONSQ_recipe.xlsx
+++ b/Brighway/Results/Lobster - CONSQ_recipe.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>('ReCiPe 2016 v1.03, midpoint (H)', 'acidification: terrestrial', 'terrestrial acidification potential (TAP)')</t>
   </si>
@@ -77,195 +77,6 @@
   </si>
   <si>
     <t>('ReCiPe 2016 v1.03, endpoint (H)', 'total: natural resources', 'natural resources')</t>
-  </si>
-  <si>
-    <t>[["Diathermy", 0.022795999451339706], ["Transport", 1.143209458023814e-05], ["Waste", 2.942409596599481e-05], ["marginal heating grid", -0.00027147224952672896], ["market for electricity, high voltage", -7.800906551536072e-05], ["erbe", 0.00020696960562547324]]</t>
-  </si>
-  <si>
-    <t>[["Diathermy", 0.011363246437063152], ["erbe", 0.00020696960562547324], ["Remanufacturing DE", 0.00021423504299291377], ["Transport", 3.1891914167260076e-05], ["Waste", 3.9158821658473844e-05], ["marginal heating grid", -0.0001357361247635117], ["market for electricity, high voltage", -3.900453275768036e-05]]</t>
-  </si>
-  <si>
-    <t>[["Autoclave (use) DK", 0.00047328920939370626], ["Bipolar burner (prod) DE", 0.00018519346089782525], ["Dishwasher (use) - DK", 0.000638740599885611], ["Scalpel (prod) DE", 0.0003819820658971264], ["Transport", 4.676204672837516e-06], ["Waste", 6.837471764850578e-06], ["marginal heating grid", -3.9940412847668846e-05], ["market for electricity, high voltage", -1.154427690932962e-05]]</t>
-  </si>
-  <si>
-    <t>[["Diathermy", 2.8387716721956298], ["Transport", 0.009325515434515421], ["Waste", 0.4270857257001284], ["marginal heating grid", -0.3293998618617417], ["market for electricity, high voltage", -0.08762786073118503], ["erbe", 0.143252448423407]]</t>
-  </si>
-  <si>
-    <t>[["Diathermy", 1.2359100509393606], ["erbe", 0.143252448423407], ["Remanufacturing DE", 0.1644467878289248], ["Transport", 0.026015227193550768], ["Waste", 0.47612660426207937], ["marginal heating grid", -0.1646999309308714], ["market for electricity, high voltage", -0.043813930365592516]]</t>
-  </si>
-  <si>
-    <t>[["Autoclave (use) DK", 0.2443698475091307], ["Bipolar burner (prod) DE", 0.05521174659371063], ["Dishwasher (use) - DK", 0.5291382578581236], ["Scalpel (prod) DE", 0.03422713734085037], ["Transport", 0.003814525723648822], ["Waste", 0.005558874362753375], ["marginal heating grid", -0.04846302521776617], ["market for electricity, high voltage", -0.01296772730925456]]</t>
-  </si>
-  <si>
-    <t>[["Diathermy", 0.7100803223028939], ["Transport", 0.00025509249346860696], ["Waste", 0.03504646889542662], ["marginal heating grid", -0.007337210497426944], ["market for electricity, high voltage", -0.0036235452871638033], ["erbe", 0.036860658178758374]]</t>
-  </si>
-  <si>
-    <t>[["Diathermy", 0.4592444212716528], ["erbe", 0.036860658178758374], ["Remanufacturing DE", 0.024268212146000334], ["Transport", 0.0007116270644290736], ["Waste", 0.035514892941760585], ["marginal heating grid", -0.003668605248715809], ["market for electricity, high voltage", -0.0018117726435819017]]</t>
-  </si>
-  <si>
-    <t>[["Autoclave (use) DK", 0.008607100698927648], ["Bipolar burner (prod) DE", 0.0032389482275325403], ["Dishwasher (use) - DK", 0.021329354689608903], ["Scalpel (prod) DE", 0.011284572413372516], ["Transport", 0.0001043434955502859], ["Waste", 0.00012282424739188037], ["marginal heating grid", -0.0010794886657077792], ["market for electricity, high voltage", -0.0005362352428165077]]</t>
-  </si>
-  <si>
-    <t>[["Diathermy", 0.9564175683523666], ["Transport", 0.0004315874696953992], ["Waste", 0.04820510442984156], ["marginal heating grid", -0.009405419539545268], ["market for electricity, high voltage", -0.004473628455151182], ["erbe", 0.044835718724945774]]</t>
-  </si>
-  <si>
-    <t>[["Diathermy", 0.6123170324989354], ["erbe", 0.044835718724945774], ["Remanufacturing DE", 0.029594059286261507], ["Transport", 0.0012039920106137717], ["Waste", 0.049174235145886105], ["marginal heating grid", -0.0047027097697755205], ["market for electricity, high voltage", -0.002236814227575591]]</t>
-  </si>
-  <si>
-    <t>[["Autoclave (use) DK", 0.011037864227658671], ["Bipolar burner (prod) DE", 0.005326334415461786], ["Dishwasher (use) - DK", 0.025822818301408885], ["Scalpel (prod) DE", 0.015642561968673113], ["Transport", 0.00017653732029267267], ["Waste", 0.00017141928500879957], ["marginal heating grid", -0.0013837743639390594], ["market for electricity, high voltage", -0.0006620359484444278]]</t>
-  </si>
-  <si>
-    <t>[["Diathermy", 150.78659218418034], ["Transport", 0.17727459857292713], ["Waste", 0.9084424412286342], ["marginal heating grid", -0.7380758595295684], ["market for electricity, high voltage", -0.22708020798318782], ["erbe", 1.3258251593541037]]</t>
-  </si>
-  <si>
-    <t>[["Diathermy", 79.32452486860748], ["erbe", 1.3258251593541037], ["Remanufacturing DE", 0.9839163765331538], ["Transport", 0.4945398449989097], ["Waste", 1.059629969694459], ["marginal heating grid", -0.3690379297648141], ["market for electricity, high voltage", -0.11354010399159391]]</t>
-  </si>
-  <si>
-    <t>[["Autoclave (use) DK", 0.738007346174707], ["Bipolar burner (prod) DE", 0.7349983715625741], ["Dishwasher (use) - DK", 1.4779551728751452], ["Scalpel (prod) DE", 3.3018513147746154], ["Transport", 0.07251272287890413], ["Waste", 0.008357757733835094], ["marginal heating grid", -0.1085895688929312], ["market for electricity, high voltage", -0.03360477124378837]]</t>
-  </si>
-  <si>
-    <t>[["Diathermy", 0.8621046839289883], ["Transport", 0.002929510915005024], ["Waste", 0.00015856342086114635], ["marginal heating grid", -0.04974439226530352], ["market for electricity, high voltage", -0.001825837773640694], ["erbe", 0.045608546433246376]]</t>
-  </si>
-  <si>
-    <t>[["Diathermy", 0.37846811753251697], ["erbe", 0.045608546433246376], ["Remanufacturing DE", 0.03710070235872109], ["Transport", 0.008172405327620627], ["Waste", 0.0009872983806865458], ["marginal heating grid", -0.02487219613265368], ["market for electricity, high voltage", -0.000912918886820347]]</t>
-  </si>
-  <si>
-    <t>[["Autoclave (use) DK", 0.06368844519615909], ["Bipolar burner (prod) DE", 0.03451029987912682], ["Dishwasher (use) - DK", 0.01714430184531586], ["Scalpel (prod) DE", 0.013747493380971663], ["Transport", 0.0011982924505853077], ["Waste", 0.00047405397583059254], ["marginal heating grid", -0.007318654364852562], ["market for electricity, high voltage", -0.0002701990686745458]]</t>
-  </si>
-  <si>
-    <t>[["Diathermy", 0.0020229571054922843], ["Transport", 9.220204030362626e-07], ["Waste", 9.600136837754658e-06], ["marginal heating grid", -2.856730770965359e-05], ["market for electricity, high voltage", -2.9850606073808963e-06], ["erbe", 1.818650114212794e-05]]</t>
-  </si>
-  <si>
-    <t>[["Diathermy", 0.0011348005060075816], ["erbe", 1.818650114212794e-05], ["Remanufacturing DE", 1.587294482355218e-05], ["Transport", 2.5721441812534555e-06], ["Waste", 1.0182434947741154e-05], ["marginal heating grid", -1.4283653854829967e-05], ["market for electricity, high voltage", -1.4925303036904481e-06]]</t>
-  </si>
-  <si>
-    <t>[["Autoclave (use) DK", 5.154175681974223e-05], ["Bipolar burner (prod) DE", 1.3098724686813556e-05], ["Dishwasher (use) - DK", 3.7163938549016964e-05], ["Scalpel (prod) DE", 2.205180277539546e-05], ["Transport", 3.771448956154962e-07], ["Waste", 2.0364396113272236e-06], ["marginal heating grid", -4.2029712645069e-06], ["market for electricity, high voltage", -4.41748225223266e-07]]</t>
-  </si>
-  <si>
-    <t>[["Diathermy", 0.00011669404471333602], ["Transport", 2.497754500498482e-07], ["Waste", 2.0324420833605896e-06], ["marginal heating grid", -2.5163792959445706e-06], ["market for electricity, high voltage", -3.1891262252801416e-07], ["erbe", 2.567041750932017e-06]]</t>
-  </si>
-  <si>
-    <t>[["Diathermy", 4.733588557028114e-05], ["erbe", 2.567041750932017e-06], ["Remanufacturing DE", 2.1395937580764564e-06], ["Transport", 6.967942014621997e-07], ["Waste", 2.1299016292443614e-06], ["marginal heating grid", -1.25818964797289e-06], ["market for electricity, high voltage", -1.5945631126400708e-07]]</t>
-  </si>
-  <si>
-    <t>[["Autoclave (use) DK", 4.6470853943823635e-06], ["Bipolar burner (prod) DE", 1.3212590569215554e-06], ["Dishwasher (use) - DK", 0.00010041200035906168], ["Scalpel (prod) DE", 1.113720179516915e-06], ["Transport", 1.0216860248012159e-07], ["Waste", 1.425733298125949e-07], ["marginal heating grid", -3.702228428015801e-07], ["market for electricity, high voltage", -4.719471512729192e-08]]</t>
-  </si>
-  <si>
-    <t>[["Diathermy", 0.22401217748020186], ["Transport", 0.00012238157028211073], ["Waste", 0.007849442019780821], ["marginal heating grid", -0.002785321186555838], ["market for electricity, high voltage", -0.001112626807663327], ["erbe", 0.006679889245152484]]</t>
-  </si>
-  <si>
-    <t>[["Diathermy", 0.11518740828435507], ["erbe", 0.006679889245152484], ["Remanufacturing DE", 0.005187674716347945], ["Transport", 0.0003414057247075094], ["Waste", 0.007459795475867526], ["marginal heating grid", -0.0013926605932769924], ["market for electricity, high voltage", -0.0005563134038316635]]</t>
-  </si>
-  <si>
-    <t>[["Autoclave (use) DK", 0.007885177647634599], ["Bipolar burner (prod) DE", 0.0022593948423794783], ["Dishwasher (use) - DK", 0.009014397567575314], ["Scalpel (prod) DE", 0.0055105781824748325], ["Transport", 5.0059179164911304e-05], ["Waste", 0.0004967905802862445], ["marginal heating grid", -0.0004097909760505699], ["market for electricity, high voltage", -0.00016465358070311497]]</t>
-  </si>
-  <si>
-    <t>[["Diathermy", 17.131718653998632], ["Transport", 0.0077777954035427276], ["Waste", 0.5608448733900042], ["marginal heating grid", -0.11065699621025192], ["market for electricity, high voltage", -0.036077084148465624], ["erbe", 0.1467455548178703]]</t>
-  </si>
-  <si>
-    <t>[["Diathermy", 10.060543865944474], ["erbe", 0.1467455548178703], ["Remanufacturing DE", 0.12016112457207374], ["Transport", 0.02169757971116636], ["Waste", 0.5526754237400845], ["marginal heating grid", -0.05532849810515969], ["market for electricity, high voltage", -0.018038542074232812]]</t>
-  </si>
-  <si>
-    <t>[["Autoclave (use) DK", 0.11732557236851504], ["Bipolar burner (prod) DE", 0.0811537765338269], ["Dishwasher (use) - DK", 0.2365581170043115], ["Scalpel (prod) DE", 0.14369693990420981], ["Transport", 0.0031814435189605065], ["Waste", 0.003190397206819988], ["marginal heating grid", -0.016280434264766285], ["market for electricity, high voltage", -0.0053389160187933705]]</t>
-  </si>
-  <si>
-    <t>[["Diathermy", 0.2111302741577785], ["Transport", 3.9977861150506413e-05], ["Waste", -0.00024938155568971843], ["marginal heating grid", -0.011287049739306073], ["market for electricity, high voltage", -1.853635412334754e-05], ["erbe", 0.0004391135304654974]]</t>
-  </si>
-  <si>
-    <t>[["Diathermy", 0.09034648594310628], ["erbe", 0.0004391135304654974], ["Remanufacturing DE", 0.0007286089974920869], ["Transport", 0.00011152553956348492], ["Waste", -0.0002635811666521836], ["marginal heating grid", -0.005643524869684946], ["market for electricity, high voltage", -9.26817706167377e-06]]</t>
-  </si>
-  <si>
-    <t>[["Autoclave (use) DK", 0.013331997262635797], ["Bipolar burner (prod) DE", 0.0023843612900236147], ["Dishwasher (use) - DK", -0.0011518325236228278], ["Scalpel (prod) DE", 0.0005655878850193272], ["Transport", 1.635261673278506e-05], ["Waste", -5.756885540670884e-05], ["marginal heating grid", -0.0016606096100372887], ["market for electricity, high voltage", -2.743127397767167e-06]]</t>
-  </si>
-  <si>
-    <t>[["Diathermy", 0.2105036308241675], ["Transport", 0.00038087301928867336], ["Waste", -0.007260797595702701], ["marginal heating grid", -0.05403592991356661], ["market for electricity, high voltage", -0.036505759175715156], ["erbe", 0.0019689460360834015]]</t>
-  </si>
-  <si>
-    <t>[["Diathermy", 0.10081405160779826], ["erbe", 0.0019689460360834015], ["Remanufacturing DE", 0.02969752667881802], ["Transport", 0.0010625147959317791], ["Waste", -0.00602031259689717], ["marginal heating grid", -0.027017964958613284], ["market for electricity, high voltage", -0.018252879587857578]]</t>
-  </si>
-  <si>
-    <t>[["Autoclave (use) DK", 0.01686404760259382], ["Bipolar burner (prod) DE", 0.0027391788057260264], ["Dishwasher (use) - DK", 0.21515760491956815], ["Scalpel (prod) DE", 0.001418969315937325], ["Transport", 0.0001557929896634683], ["Waste", 0.00019547718257482402], ["marginal heating grid", -0.007950047756343144], ["market for electricity, high voltage", -0.00540235407161421]]</t>
-  </si>
-  <si>
-    <t>[["Diathermy", -0.04188596592598191], ["Transport", 3.981534377599031e-05], ["Waste", -4.4835508899238864e-05], ["marginal heating grid", -0.00017562303513900645], ["market for electricity, high voltage", -9.622316129383784e-05], ["erbe", 0.00037138901367539894]]</t>
-  </si>
-  <si>
-    <t>[["Diathermy", -0.014285282709193197], ["erbe", 0.00037138901367539894], ["Remanufacturing DE", 0.00029325122137091814], ["Transport", 0.00011107216768583086], ["Waste", -2.373752138413633e-05], ["marginal heating grid", -8.781151757217059e-05], ["market for electricity, high voltage", -4.811158064691892e-05]]</t>
-  </si>
-  <si>
-    <t>[["Autoclave (use) DK", 0.0002965053602764305], ["Bipolar burner (prod) DE", 2.6011686841008736e-05], ["Dishwasher (use) - DK", 0.0006360922272424508], ["Scalpel (prod) DE", 0.002560434762295338], ["Transport", 1.628614033086374e-05], ["Waste", 4.4771722169544e-06], ["marginal heating grid", -2.5838576655958074e-05], ["market for electricity, high voltage", -1.4239714470736933e-05]]</t>
-  </si>
-  <si>
-    <t>[["Diathermy", 3.1623708960471428e-06], ["Transport", 4.101500207581304e-09], ["Waste", 7.59433070845262e-08], ["marginal heating grid", -8.749365178855315e-08], ["market for electricity, high voltage", -3.5050423688620864e-08], ["erbe", 8.702010013262805e-08]]</t>
-  </si>
-  <si>
-    <t>[["Diathermy", 5.691369882312088e-07], ["erbe", 8.702010013262805e-08], ["Remanufacturing DE", 7.882216407238434e-08], ["Transport", 1.1441883345093026e-08], ["Waste", 7.881839801496722e-08], ["marginal heating grid", -4.374682589427102e-08], ["market for electricity, high voltage", -1.7525211844310432e-08]]</t>
-  </si>
-  <si>
-    <t>[["Autoclave (use) DK", 4.7714963169403366e-08], ["Bipolar burner (prod) DE", 1.3879690257216751e-08], ["Dishwasher (use) - DK", 3.6303783317318507e-07], ["Scalpel (prod) DE", 8.269532757953126e-09], ["Transport", 1.6776850735204796e-09], ["Waste", 8.895406646983889e-10], ["marginal heating grid", -1.2872522256255399e-08], ["market for electricity, high voltage", -5.186984284168736e-09]]</t>
-  </si>
-  <si>
-    <t>[["Diathermy", 0.009479150001862714], ["Transport", 7.046592384038083e-06], ["Waste", 1.6555080448302415e-05], ["marginal heating grid", -0.00016604015769895928], ["market for electricity, high voltage", -2.7508858293943308e-05], ["erbe", 9.284490485619051e-05]]</t>
-  </si>
-  <si>
-    <t>[["Diathermy", 0.004591644798391262], ["erbe", 9.284490485619051e-05], ["Remanufacturing DE", 9.276774394118946e-05], ["Transport", 1.9657755445087838e-05], ["Waste", 2.041227720207364e-05], ["marginal heating grid", -8.302007884951996e-05], ["market for electricity, high voltage", -1.3754429146971654e-05]]</t>
-  </si>
-  <si>
-    <t>[["Autoclave (use) DK", 0.00020963795005238722], ["Bipolar burner (prod) DE", 7.505294983830652e-05], ["Dishwasher (use) - DK", 0.0002622699725493933], ["Scalpel (prod) DE", 0.00015082314906719721], ["Transport", 2.8823509115104234e-06], ["Waste", 3.963032337426284e-06], ["marginal heating grid", -2.4428693759136836e-05], ["market for electricity, high voltage", -4.070935544564964e-06]]</t>
-  </si>
-  <si>
-    <t>[["Diathermy", 0.008492452404010597], ["Transport", 1.4617259240420664e-05], ["Waste", 5.543066643514747e-05], ["marginal heating grid", -0.0003622686231928102], ["market for electricity, high voltage", -9.108435277566031e-05], ["erbe", 0.00019373024957536144]]</t>
-  </si>
-  <si>
-    <t>[["Diathermy", 0.004007765056050113], ["erbe", 0.00019373024957536144], ["Remanufacturing DE", 0.0002103855349829359], ["Transport", 4.077751227338234e-05], ["Waste", 6.924906884596891e-05], ["marginal heating grid", -0.00018113431159641862], ["market for electricity, high voltage", -4.5542176387830156e-05]]</t>
-  </si>
-  <si>
-    <t>[["Autoclave (use) DK", 0.0003181866186194646], ["Bipolar burner (prod) DE", 0.00011374561636475346], ["Dishwasher (use) - DK", 0.0005578926404596333], ["Scalpel (prod) DE", 9.452488435001651e-05], ["Transport", 5.97907019438922e-06], ["Waste", 3.5148294245067042e-06], ["marginal heating grid", -5.3298848767486176e-05], ["market for electricity, high voltage", -1.3479240952351127e-05]]</t>
-  </si>
-  <si>
-    <t>[["Diathermy", 0.008768906997631413], ["Transport", 1.6594221735862795e-05], ["Waste", 5.350248185623578e-05], ["marginal heating grid", -0.00038284856643518953], ["market for electricity, high voltage", -9.308446286476392e-05], ["erbe", 0.00021322885266393264]]</t>
-  </si>
-  <si>
-    <t>[["Diathermy", 0.00413763778582307], ["erbe", 0.00021322885266393264], ["Remanufacturing DE", 0.00022544040336855843], ["Transport", 4.629260994634321e-05], ["Waste", 6.799507859583741e-05], ["marginal heating grid", -0.00019142428321760867], ["market for electricity, high voltage", -4.654223143238196e-05]]</t>
-  </si>
-  <si>
-    <t>[["Autoclave (use) DK", 0.00034266591443511826], ["Bipolar burner (prod) DE", 0.0001226407335679011], ["Dishwasher (use) - DK", 0.00057772888219192], ["Scalpel (prod) DE", 9.963035979470777e-05], ["Transport", 6.787730514186848e-06], ["Waste", 3.7229815808947703e-06], ["marginal heating grid", -5.632667732423958e-05], ["market for electricity, high voltage", -1.3775229944979313e-05]]</t>
-  </si>
-  <si>
-    <t>[["Diathermy", 0.017183667963708835], ["Transport", 1.3643310382892691e-05], ["Waste", 0.0004840761415572034], ["marginal heating grid", -0.00047935345373705917], ["market for electricity, high voltage", -8.102697277740707e-05], ["erbe", 0.0004354443458863415]]</t>
-  </si>
-  <si>
-    <t>[["Diathermy", 0.006849868124472102], ["erbe", 0.0004354443458863415], ["Remanufacturing DE", 0.0005208413367777552], ["Transport", 3.8060504191476985e-05], ["Waste", 0.0004983730415622475], ["marginal heating grid", -0.0002396767268685848], ["market for electricity, high voltage", -4.0513486388703534e-05]]</t>
-  </si>
-  <si>
-    <t>[["Autoclave (use) DK", 0.00050314533497959], ["Bipolar burner (prod) DE", 0.0007218761707038871], ["Dishwasher (use) - DK", 0.003502276673167414], ["Scalpel (prod) DE", 0.00018008860278806937], ["Transport", 5.58068438969563e-06], ["Waste", 2.9005553742863094e-05], ["marginal heating grid", -7.05249795351731e-05], ["market for electricity, high voltage", -1.1990885991102152e-05]]</t>
-  </si>
-  <si>
-    <t>[["Diathermy", 1.9451248543312664e-08], ["Transport", 3.692304290340566e-11], ["Waste", 1.1907824913738393e-09], ["marginal heating grid", -1.5421505427572035e-09], ["market for electricity, high voltage", -6.051776200711805e-10], ["erbe", 5.475881521516752e-10]]</t>
-  </si>
-  <si>
-    <t>[["Diathermy", 9.34694300087397e-09], ["erbe", 5.475881521516752e-10], ["Remanufacturing DE", 8.401264846724101e-10], ["Transport", 1.0300356656487296e-10], ["Waste", 1.3455831292844273e-09], ["marginal heating grid", -7.71075271394885e-10], ["market for electricity, high voltage", -3.0258881003559023e-10]]</t>
-  </si>
-  <si>
-    <t>[["Autoclave (use) DK", 1.0285104732355619e-09], ["Bipolar burner (prod) DE", 2.5399663714233244e-10], ["Dishwasher (use) - DK", 3.659448262061686e-09], ["Scalpel (prod) DE", 2.642279759828031e-10], ["Transport", 1.5103068344158015e-11], ["Waste", 2.0792311770682083e-11], ["marginal heating grid", -2.2688922882052948e-10], ["market for electricity, high voltage", -8.955802738150805e-11]]</t>
-  </si>
-  <si>
-    <t>[["Diathermy", 1.3286877754842911e-05], ["Transport", 1.530961925420887e-08], ["Waste", 5.619134215521335e-07], ["marginal heating grid", -4.4608658984028295e-07], ["market for electricity, high voltage", -1.108183974600807e-07], ["erbe", 2.480948849802798e-07]]</t>
-  </si>
-  <si>
-    <t>[["Diathermy", 6.726897973464541e-06], ["erbe", 2.480948849802798e-07], ["Remanufacturing DE", 2.569173913623242e-07], ["Transport", 4.270897688624063e-08], ["Waste", 6.067348065827113e-07], ["marginal heating grid", -2.2304329492017229e-07], ["market for electricity, high voltage", -5.540919873004035e-08]]</t>
-  </si>
-  <si>
-    <t>[["Autoclave (use) DK", 4.129587297324633e-07], ["Bipolar burner (prod) DE", 1.2611679918946047e-07], ["Dishwasher (use) - DK", 7.482905480719234e-07], ["Scalpel (prod) DE", 1.7806415276832804e-07], ["Transport", 6.262274388427491e-09], ["Waste", 1.0094391448504076e-08], ["marginal heating grid", -6.563058506019625e-08], ["market for electricity, high voltage", -1.639961020524467e-08]]</t>
-  </si>
-  <si>
-    <t>[["Diathermy", 0.2261517424936987], ["Transport", 0.0012339467108585258], ["Waste", -0.00012786992775163926], ["marginal heating grid", -0.016975226321806144], ["market for electricity, high voltage", -0.0006065841339330884], ["erbe", 0.016065681328172283]]</t>
-  </si>
-  <si>
-    <t>[["Diathermy", 0.09882208338617243], ["erbe", 0.016065681328172283], ["Remanufacturing DE", 0.013413761947450732], ["Transport", 0.0034423195428856224], ["Waste", 0.00017930474705875327], ["marginal heating grid", -0.008487613160904092], ["market for electricity, high voltage", -0.0003032920669665442]]</t>
-  </si>
-  <si>
-    <t>[["Autoclave (use) DK", 0.021233241421315788], ["Bipolar burner (prod) DE", 0.013547169843528498], ["Dishwasher (use) - DK", 0.004934718284916485], ["Scalpel (prod) DE", 0.005152377735126872], ["Transport", 0.0005047357975259237], ["Waste", 0.00015758609064746656], ["marginal heating grid", -0.002497483807860451], ["market for electricity, high voltage", -8.976617223482518e-05]]</t>
   </si>
 </sst>
 </file>
@@ -623,7 +434,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -694,201 +505,6 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
-      <c r="A2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" t="s">
-        <v>42</v>
-      </c>
-      <c r="I2" t="s">
-        <v>45</v>
-      </c>
-      <c r="J2" t="s">
-        <v>48</v>
-      </c>
-      <c r="K2" t="s">
-        <v>51</v>
-      </c>
-      <c r="L2" t="s">
-        <v>54</v>
-      </c>
-      <c r="M2" t="s">
-        <v>57</v>
-      </c>
-      <c r="N2" t="s">
-        <v>60</v>
-      </c>
-      <c r="O2" t="s">
-        <v>63</v>
-      </c>
-      <c r="P2" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>69</v>
-      </c>
-      <c r="R2" t="s">
-        <v>72</v>
-      </c>
-      <c r="S2" t="s">
-        <v>75</v>
-      </c>
-      <c r="T2" t="s">
-        <v>78</v>
-      </c>
-      <c r="U2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H3" t="s">
-        <v>43</v>
-      </c>
-      <c r="I3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J3" t="s">
-        <v>49</v>
-      </c>
-      <c r="K3" t="s">
-        <v>52</v>
-      </c>
-      <c r="L3" t="s">
-        <v>55</v>
-      </c>
-      <c r="M3" t="s">
-        <v>58</v>
-      </c>
-      <c r="N3" t="s">
-        <v>61</v>
-      </c>
-      <c r="O3" t="s">
-        <v>64</v>
-      </c>
-      <c r="P3" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>70</v>
-      </c>
-      <c r="R3" t="s">
-        <v>73</v>
-      </c>
-      <c r="S3" t="s">
-        <v>76</v>
-      </c>
-      <c r="T3" t="s">
-        <v>79</v>
-      </c>
-      <c r="U3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" t="s">
-        <v>44</v>
-      </c>
-      <c r="I4" t="s">
-        <v>47</v>
-      </c>
-      <c r="J4" t="s">
-        <v>50</v>
-      </c>
-      <c r="K4" t="s">
-        <v>53</v>
-      </c>
-      <c r="L4" t="s">
-        <v>56</v>
-      </c>
-      <c r="M4" t="s">
-        <v>59</v>
-      </c>
-      <c r="N4" t="s">
-        <v>62</v>
-      </c>
-      <c r="O4" t="s">
-        <v>65</v>
-      </c>
-      <c r="P4" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>71</v>
-      </c>
-      <c r="R4" t="s">
-        <v>74</v>
-      </c>
-      <c r="S4" t="s">
-        <v>77</v>
-      </c>
-      <c r="T4" t="s">
-        <v>80</v>
-      </c>
-      <c r="U4" t="s">
-        <v>83</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>